<commit_message>
final attempt. couldn't figure out add_desktop
</commit_message>
<xml_diff>
--- a/elsa/Scrum_ELSA.xlsx
+++ b/elsa/Scrum_ELSA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28785" windowHeight="12840" tabRatio="500"/>
+    <workbookView windowWidth="28785" windowHeight="12840" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="88">
   <si>
     <t>Product Name:</t>
   </si>
@@ -217,6 +217,9 @@
     <t>Write the Customer class</t>
   </si>
   <si>
+    <t>Completed Day 7</t>
+  </si>
+  <si>
     <t>Test each class and method as it is written</t>
   </si>
   <si>
@@ -253,6 +256,9 @@
     <t>Write the Order associative class and constructor</t>
   </si>
   <si>
+    <t>also added operator overload for Order</t>
+  </si>
+  <si>
     <t>Write Order::add_product</t>
   </si>
   <si>
@@ -262,7 +268,16 @@
     <t>Write Store::new_order, add_desktop, num_orders, and order</t>
   </si>
   <si>
+    <t>In Work</t>
+  </si>
+  <si>
+    <t>didn't complete add_desktop, everything else should be done</t>
+  </si>
+  <si>
     <t>Integrate and test with cse1325_prof/elsa/sprint_1/main.cpp</t>
+  </si>
+  <si>
+    <t>could not test because add_desktop function was missing.</t>
   </si>
   <si>
     <t>Ensure ALL CODE is on GitHub by deadline!</t>
@@ -276,14 +291,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="176" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
+    <numFmt numFmtId="177" formatCode="mmm\ dd"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
-    <numFmt numFmtId="177" formatCode="mmm\ dd"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="30">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -351,16 +366,26 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -373,23 +398,46 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -402,9 +450,24 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -422,29 +485,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -461,44 +509,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -525,7 +535,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,19 +571,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,73 +607,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -645,49 +637,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -705,7 +661,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -758,6 +768,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -769,39 +794,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -845,151 +842,164 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1764,7 +1774,7 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3985,7 +3995,7 @@
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A10" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -5436,13 +5446,13 @@
       <formula1>"0,1,2,3,5,8,13,21,34,55,89"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Initials" prompt="Please enter 2 or 3 capital letters that will represent you  in the &quot;Assigned To&quot; column on each Sprint Backlog tab of this spreadsheet." sqref="H5"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Name" prompt="Select any team name you prefer." sqref="B2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Max Bonus Points" prompt="This is the MAXIMUM number of bonus points awarded if you successfully and completely implement this feature.&#10;&#10;If blank, this feature is REQUIRED. You MAY NOT work on ANY bonus feature until ALL required features have been implemented.&#10;&#10;If non-blank, some or all bonus points will be awarded ONLY if the feature is COMPLETELY implemented.&#10; Complete but non-optimal implementations may receive partial credit. &#10;Incomplete or nearly-complete implementations will receive no bonus points." sqref="D24:D96"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Name" prompt="Please enter your name as it appears in Blackboard." sqref="B5"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Student ID" prompt="Please enter your UTA student ID number." sqref="I5"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Initials" prompt="Please enter 2 or 3 capital letters that will represent you  in the &quot;Assigned To&quot; column on each Sprint Backlog tab of this spreadsheet." sqref="H5"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Relative Priority" prompt="This is the priority ranking for this feature, relative to all other features.&#10;&#10;Lower integers are higher in prioirty.&#10;&#10;The customer may add or (for unimplemented features) remove features and change priority rankings at the start of each sprint." sqref="B24:B96"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Required Sprint" prompt="This is the sprint during which the grader will grade your implementation of this feature.&#10;&#10;By the END of this sprint, you must have implemented this feature.&#10;&#10;If this field is blank, then this is a bonus feature. If implemented, it will be graded after the final sprint for extra credit." sqref="C24:C96"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Max Bonus Points" prompt="This is the MAXIMUM number of bonus points awarded if you successfully and completely implement this feature.&#10;&#10;If blank, this feature is REQUIRED. You MAY NOT work on ANY bonus feature until ALL required features have been implemented.&#10;&#10;If non-blank, some or all bonus points will be awarded ONLY if the feature is COMPLETELY implemented.&#10; Complete but non-optimal implementations may receive partial credit. &#10;Incomplete or nearly-complete implementations will receive no bonus points." sqref="D24:D96"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Sprint" prompt="Select the sprint number (1, 2, etc.) in which you plan to implement this feature.  This is just for planning purposes, it won't affect your grade.&#10;&#10;In Scrum, you only plan the current sprint, not future sprints, so you don't need to fill this in for any features not planned for the current sprint.&#10;&#10;If you planned a &quot;full credit&quot; feature for the current sprint but don't complete it, then just update this cell for the next sprint.  This will only affect your grade if this feature was *required* to be completed by a specific sprint, and is not.&#10;&#10;If you planned a &quot;bonus&quot; or &quot;extreme bonus&quot; feature for the current sprint but don't complete it, and you don't want to use it for the next sprint, just use the Delete key to leave this cell blank. Your &quot;full credit&quot; grade will not be penalized for this decision." sqref="F24:F96">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
@@ -5471,8 +5481,8 @@
   <sheetPr/>
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -5700,11 +5710,11 @@
       </c>
       <c r="B14" s="2">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(E$17:E$995,"Completed Day 7")</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -5752,9 +5762,11 @@
       <c r="D17" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="11"/>
+      <c r="E17" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="F17" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -5765,11 +5777,13 @@
         <v>32</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="11"/>
+        <v>67</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="F18" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -5780,9 +5794,11 @@
         <v>32</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="11"/>
+        <v>69</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6">
@@ -5793,9 +5809,11 @@
         <v>37</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="11"/>
+        <v>70</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6">
@@ -5806,9 +5824,11 @@
         <v>37</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="11"/>
+        <v>71</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="F21" s="12"/>
     </row>
     <row r="22" spans="1:6">
@@ -5819,9 +5839,11 @@
         <v>37</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="11"/>
+        <v>72</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:6">
@@ -5832,9 +5854,11 @@
         <v>41</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E23" s="11"/>
+        <v>73</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="F23" s="12"/>
     </row>
     <row r="24" spans="1:6">
@@ -5845,9 +5869,11 @@
         <v>41</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" s="11"/>
+        <v>74</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="F24" s="12"/>
     </row>
     <row r="25" spans="1:6">
@@ -5858,9 +5884,11 @@
         <v>41</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="E25" s="11"/>
+        <v>75</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:6">
@@ -5871,9 +5899,11 @@
         <v>41</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" s="11"/>
+        <v>76</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="F26" s="12"/>
     </row>
     <row r="27" spans="1:6">
@@ -5884,10 +5914,14 @@
         <v>44</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="12"/>
+        <v>77</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28">
@@ -5897,9 +5931,11 @@
         <v>44</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" s="11"/>
+        <v>79</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="F28" s="12"/>
     </row>
     <row r="29" spans="1:6">
@@ -5910,9 +5946,11 @@
         <v>44</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E29" s="11"/>
+        <v>80</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="F29" s="12"/>
     </row>
     <row r="30" spans="1:6">
@@ -5923,10 +5961,14 @@
         <v>44</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="12"/>
+        <v>81</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31">
@@ -5936,10 +5978,14 @@
         <v>44</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31" s="11"/>
-      <c r="F31" s="12"/>
+        <v>84</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32">
@@ -5949,9 +5995,11 @@
         <v>44</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E32" s="11"/>
+        <v>86</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="F32" s="12"/>
     </row>
     <row r="33" spans="1:6">
@@ -6568,9 +6616,9 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the manual to cover this feature&quot;, or &quot;Fix the seg fault bug&quot;.&#10;&#10;Expect roughly 3 to 10 tasks per typical feature. Don't OVER plan, but also don't just write &quot;Implement the feature&quot;. Find a middle ground. :-)" sqref="D17:D100"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task ID" prompt="This is just an arbitrary unique (per sprint) integer assigned to a task, used by the team to refer to that task. " sqref="A17:A100"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="The list contains the Feature IDs from the same column on the Product Backlog tab.&#10;&#10;For each (ahem) Feature ID, create one or more rows in this table representing the tasks you need to complete to implement that feature.&#10;&#10;For example, for a &quot;Provide Help to User&quot; feature, you might assign a Feature ID of &quot;HELP&quot; on the Product Backlog. Then, in the Sprint Backlog table, you might have 3 rows of tasks with Feature ID of Help - &quot;Write help text&quot;, &quot;Create help class to display help&quot;, and &quot;Update CLI to accept '?' command&quot;.&#10;&#10;COPY the status cell from row 1 for each row that you add, so that you can select its status with a drop-down. This will ensure that the Sprint Burn Chart at the top updates itself automatically as you complete your tasks." sqref="B17:B100">
       <formula1>'Product Backlog'!$A$24:$A$96</formula1>
     </dataValidation>
@@ -6875,7 +6923,7 @@
       </c>
       <c r="B17" s="9"/>
       <c r="D17" s="10" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="12"/>
@@ -7629,9 +7677,9 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the manual to cover this feature&quot;, or &quot;Fix the seg fault bug&quot;.&#10;&#10;Expect roughly 3 to 10 tasks per typical feature. Don't OVER plan, but also don't just write &quot;Implement the feature&quot;. Find a middle ground. :-)" sqref="D18:D100"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task ID" prompt="This is just an arbitrary unique (per sprint) integer assigned to a task, used by the team to refer to that task. " sqref="A17:A100"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="The list contains the Feature IDs from the same column on the Product Backlog tab.&#10;&#10;For each (ahem) Feature ID, create one or more rows in this table representing the tasks you need to complete to implement that feature.&#10;&#10;For example, for a &quot;Provide Help to User&quot; feature, you might assign a Feature ID of &quot;HELP&quot; on the Product Backlog. Then, in the Sprint Backlog table, you might have 3 rows of tasks with Feature ID of Help - &quot;Write help text&quot;, &quot;Create help class to display help&quot;, and &quot;Update CLI to accept '?' command&quot;.&#10;&#10;COPY the status cell from row 1 for each row that you add, so that you can select its status with a drop-down. This will ensure that the Sprint Burn Chart at the top updates itself automatically as you complete your tasks." sqref="B17:B100">
       <formula1>'Product Backlog'!$A$24:$A$96</formula1>
     </dataValidation>
@@ -7936,7 +7984,7 @@
       </c>
       <c r="B17" s="9"/>
       <c r="D17" s="10" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="12"/>
@@ -8690,9 +8738,9 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the manual to cover this feature&quot;, or &quot;Fix the seg fault bug&quot;.&#10;&#10;Expect roughly 3 to 10 tasks per typical feature. Don't OVER plan, but also don't just write &quot;Implement the feature&quot;. Find a middle ground. :-)" sqref="D18:D100"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task ID" prompt="This is just an arbitrary unique (per sprint) integer assigned to a task, used by the team to refer to that task. " sqref="A17:A100"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="The list contains the Feature IDs from the same column on the Product Backlog tab.&#10;&#10;For each (ahem) Feature ID, create one or more rows in this table representing the tasks you need to complete to implement that feature.&#10;&#10;For example, for a &quot;Provide Help to User&quot; feature, you might assign a Feature ID of &quot;HELP&quot; on the Product Backlog. Then, in the Sprint Backlog table, you might have 3 rows of tasks with Feature ID of Help - &quot;Write help text&quot;, &quot;Create help class to display help&quot;, and &quot;Update CLI to accept '?' command&quot;.&#10;&#10;COPY the status cell from row 1 for each row that you add, so that you can select its status with a drop-down. This will ensure that the Sprint Burn Chart at the top updates itself automatically as you complete your tasks." sqref="B17:B100">
       <formula1>'Product Backlog'!$A$24:$A$96</formula1>
     </dataValidation>
@@ -8997,7 +9045,7 @@
       </c>
       <c r="B17" s="9"/>
       <c r="D17" s="10" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="12"/>
@@ -9751,9 +9799,9 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the manual to cover this feature&quot;, or &quot;Fix the seg fault bug&quot;.&#10;&#10;Expect roughly 3 to 10 tasks per typical feature. Don't OVER plan, but also don't just write &quot;Implement the feature&quot;. Find a middle ground. :-)" sqref="D18:D100"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task ID" prompt="This is just an arbitrary unique (per sprint) integer assigned to a task, used by the team to refer to that task. " sqref="A17:A100"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="The list contains the Feature IDs from the same column on the Product Backlog tab.&#10;&#10;For each (ahem) Feature ID, create one or more rows in this table representing the tasks you need to complete to implement that feature.&#10;&#10;For example, for a &quot;Provide Help to User&quot; feature, you might assign a Feature ID of &quot;HELP&quot; on the Product Backlog. Then, in the Sprint Backlog table, you might have 3 rows of tasks with Feature ID of Help - &quot;Write help text&quot;, &quot;Create help class to display help&quot;, and &quot;Update CLI to accept '?' command&quot;.&#10;&#10;COPY the status cell from row 1 for each row that you add, so that you can select its status with a drop-down. This will ensure that the Sprint Burn Chart at the top updates itself automatically as you complete your tasks." sqref="B17:B100">
       <formula1>'Product Backlog'!$A$24:$A$96</formula1>
     </dataValidation>
@@ -10058,7 +10106,7 @@
       </c>
       <c r="B17" s="9"/>
       <c r="D17" s="10" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="12"/>
@@ -10812,9 +10860,9 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the manual to cover this feature&quot;, or &quot;Fix the seg fault bug&quot;.&#10;&#10;Expect roughly 3 to 10 tasks per typical feature. Don't OVER plan, but also don't just write &quot;Implement the feature&quot;. Find a middle ground. :-)" sqref="D18:D100"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task ID" prompt="This is just an arbitrary unique (per sprint) integer assigned to a task, used by the team to refer to that task. " sqref="A17:A100"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="The list contains the Feature IDs from the same column on the Product Backlog tab.&#10;&#10;For each (ahem) Feature ID, create one or more rows in this table representing the tasks you need to complete to implement that feature.&#10;&#10;For example, for a &quot;Provide Help to User&quot; feature, you might assign a Feature ID of &quot;HELP&quot; on the Product Backlog. Then, in the Sprint Backlog table, you might have 3 rows of tasks with Feature ID of Help - &quot;Write help text&quot;, &quot;Create help class to display help&quot;, and &quot;Update CLI to accept '?' command&quot;.&#10;&#10;COPY the status cell from row 1 for each row that you add, so that you can select its status with a drop-down. This will ensure that the Sprint Burn Chart at the top updates itself automatically as you complete your tasks." sqref="B17:B100">
       <formula1>'Product Backlog'!$A$24:$A$96</formula1>
     </dataValidation>

</xml_diff>